<commit_message>
Add enough test SNAP data to support running 5 bins
</commit_message>
<xml_diff>
--- a/tests/resources/SNAP_2019_test.xlsx
+++ b/tests/resources/SNAP_2019_test.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <t xml:space="preserve">White</t>
   </si>
@@ -47,6 +47,21 @@
   </si>
   <si>
     <t xml:space="preserve">ADAMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALEXANDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BROWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUREAU</t>
   </si>
   <si>
     <t xml:space="preserve">Sum:</t>
@@ -362,11 +377,11 @@
   </sheetPr>
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="3:103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="8:103 A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -418,50 +433,135 @@
         <v>516</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>371</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>49</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>188</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>297</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>68</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>213</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
@@ -1327,14 +1427,31 @@
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="6"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
+    <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" s="5" t="n">
+        <v>66186</v>
+      </c>
+      <c r="C104" s="5" t="n">
+        <v>51936</v>
+      </c>
+      <c r="D104" s="5" t="n">
+        <v>557</v>
+      </c>
+      <c r="E104" s="5" t="n">
+        <v>2936</v>
+      </c>
+      <c r="F104" s="5" t="n">
+        <v>415</v>
+      </c>
+      <c r="G104" s="5" t="n">
+        <v>32471</v>
+      </c>
+      <c r="H104" s="0" t="n">
+        <v>91836</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1"/>
@@ -1381,11 +1498,11 @@
   </sheetPr>
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="3:103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A103" activeCellId="0" sqref="8:103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.48046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.4609375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="1" style="7" width="18.44"/>
   </cols>
@@ -1440,50 +1557,135 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>127</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>320</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>796</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>418</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>109</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>593</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>126</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>546</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
@@ -2349,14 +2551,31 @@
       <c r="G103" s="5"/>
       <c r="H103" s="5"/>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="6"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
+    <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" s="5" t="n">
+        <v>137609</v>
+      </c>
+      <c r="C104" s="1" t="n">
+        <v>88743</v>
+      </c>
+      <c r="D104" s="1" t="n">
+        <v>1144</v>
+      </c>
+      <c r="E104" s="7" t="n">
+        <v>6029</v>
+      </c>
+      <c r="F104" s="5" t="n">
+        <v>590</v>
+      </c>
+      <c r="G104" s="5" t="n">
+        <v>73029</v>
+      </c>
+      <c r="H104" s="5" t="n">
+        <v>259298</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1"/>
@@ -2392,11 +2611,11 @@
   </sheetPr>
   <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A109" activeCellId="1" sqref="3:103 A109"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="8:103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="7" width="16.56"/>
   </cols>
@@ -2511,55 +2730,135 @@
         <v>295</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>473</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>475</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>936</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>74</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>2046</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>205</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>403</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>291</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>142</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
@@ -3523,7 +3822,7 @@
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B110" s="5" t="n">
         <v>399790</v>
@@ -3580,15 +3879,15 @@
   </sheetPr>
   <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="7" width="38.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="7" width="9.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="7" width="9.11"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3641,54 +3940,134 @@
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>84</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>78</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>130</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>366</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>127</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
@@ -4652,7 +5031,7 @@
     </row>
     <row r="104" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B104" s="5" t="n">
         <v>78782</v>

</xml_diff>

<commit_message>
Add Bins to SNAP Participation Data (#69)
* Add enough test SNAP data to support running 5 bins

* First pass at adding metrics

* Fix bin names to match data names for age groups

* Add quantiles bins

* Refactor the binning into a function to make the main snap runner function simpler

* Fix flake8 errors

* Refactor rename_columns() to be more idiomatic

* Make make_bins Doc String Match the Formatting of the File
</commit_message>
<xml_diff>
--- a/tests/resources/SNAP_2019_test.xlsx
+++ b/tests/resources/SNAP_2019_test.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <t xml:space="preserve">White</t>
   </si>
@@ -47,6 +47,21 @@
   </si>
   <si>
     <t xml:space="preserve">ADAMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALEXANDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BROWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUREAU</t>
   </si>
   <si>
     <t xml:space="preserve">Sum:</t>
@@ -362,11 +377,11 @@
   </sheetPr>
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="3:103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="8:103 A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -418,50 +433,135 @@
         <v>516</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>371</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>49</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>188</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>297</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>68</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>213</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
@@ -1327,14 +1427,31 @@
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="6"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
+    <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" s="5" t="n">
+        <v>66186</v>
+      </c>
+      <c r="C104" s="5" t="n">
+        <v>51936</v>
+      </c>
+      <c r="D104" s="5" t="n">
+        <v>557</v>
+      </c>
+      <c r="E104" s="5" t="n">
+        <v>2936</v>
+      </c>
+      <c r="F104" s="5" t="n">
+        <v>415</v>
+      </c>
+      <c r="G104" s="5" t="n">
+        <v>32471</v>
+      </c>
+      <c r="H104" s="0" t="n">
+        <v>91836</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1"/>
@@ -1381,11 +1498,11 @@
   </sheetPr>
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="3:103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A103" activeCellId="0" sqref="8:103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.48046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.4609375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="1" style="7" width="18.44"/>
   </cols>
@@ -1440,50 +1557,135 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>127</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>320</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>796</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>418</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>109</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>593</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>126</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>546</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
@@ -2349,14 +2551,31 @@
       <c r="G103" s="5"/>
       <c r="H103" s="5"/>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="6"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
+    <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" s="5" t="n">
+        <v>137609</v>
+      </c>
+      <c r="C104" s="1" t="n">
+        <v>88743</v>
+      </c>
+      <c r="D104" s="1" t="n">
+        <v>1144</v>
+      </c>
+      <c r="E104" s="7" t="n">
+        <v>6029</v>
+      </c>
+      <c r="F104" s="5" t="n">
+        <v>590</v>
+      </c>
+      <c r="G104" s="5" t="n">
+        <v>73029</v>
+      </c>
+      <c r="H104" s="5" t="n">
+        <v>259298</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1"/>
@@ -2392,11 +2611,11 @@
   </sheetPr>
   <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A109" activeCellId="1" sqref="3:103 A109"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="8:103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="7" width="16.56"/>
   </cols>
@@ -2511,55 +2730,135 @@
         <v>295</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>473</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>475</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>936</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>74</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>2046</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>205</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>403</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>291</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>90</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>142</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
@@ -3523,7 +3822,7 @@
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B110" s="5" t="n">
         <v>399790</v>
@@ -3580,15 +3879,15 @@
   </sheetPr>
   <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="8:103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="7" width="38.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="7" width="9.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="7" width="9.11"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3641,54 +3940,134 @@
       </c>
     </row>
     <row r="3" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>84</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>78</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>130</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>366</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>127</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
@@ -4652,7 +5031,7 @@
     </row>
     <row r="104" s="1" customFormat="true" ht="19.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B104" s="5" t="n">
         <v>78782</v>

</xml_diff>